<commit_message>
Removed 0 for missing ratings.
</commit_message>
<xml_diff>
--- a/pagelle.xlsx
+++ b/pagelle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M\OneDrive\GIT\j\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5279EDBC-9E37-48A5-8228-8A47A1A77365}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A8DAC01B-50E6-4B50-A65A-7A4264AD0500}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="4" xr2:uid="{B3A0D2B9-F8C4-4AFA-8483-391A4991D9E4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{B3A0D2B9-F8C4-4AFA-8483-391A4991D9E4}"/>
   </bookViews>
   <sheets>
     <sheet name="DBNotes" sheetId="1" r:id="rId1"/>
@@ -941,11 +941,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CFEFEF-989E-47C9-ACC2-19406C570125}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,15 +1561,6 @@
       <c r="G14">
         <v>5.5</v>
       </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
       <c r="K14">
         <v>5.5</v>
       </c>
@@ -1578,9 +1569,6 @@
       </c>
       <c r="M14">
         <v>6</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1602,29 +1590,8 @@
       <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
       <c r="M15">
         <v>5.5</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1649,17 +1616,8 @@
       <c r="G16">
         <v>6</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
         <v>6</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
       </c>
       <c r="L16">
         <v>6</v>
@@ -2174,23 +2132,11 @@
       <c r="F28" t="s">
         <v>34</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
       <c r="H28">
         <v>6</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>6</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
       </c>
       <c r="M28">
         <v>6.5</v>
@@ -2309,9 +2255,6 @@
       <c r="G31">
         <v>6</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
       <c r="I31">
         <v>6.5</v>
       </c>
@@ -2762,23 +2705,8 @@
       <c r="F43" t="s">
         <v>44</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
       <c r="L43">
         <v>6</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -2879,9 +2807,6 @@
       <c r="G46">
         <v>6.5</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
       <c r="I46">
         <v>7</v>
       </c>
@@ -3370,23 +3295,8 @@
       <c r="F59" t="s">
         <v>57</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <v>0</v>
-      </c>
       <c r="L59">
         <v>5.5</v>
-      </c>
-      <c r="M59">
-        <v>0</v>
-      </c>
-      <c r="N59">
-        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -3449,9 +3359,6 @@
       <c r="G61">
         <v>5.5</v>
       </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
       <c r="I61">
         <v>6</v>
       </c>
@@ -3902,24 +3809,6 @@
       <c r="F73" t="s">
         <v>108</v>
       </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-      <c r="M73">
-        <v>0</v>
-      </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -3946,9 +3835,6 @@
       <c r="H74">
         <v>6</v>
       </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
       <c r="L74">
         <v>6</v>
       </c>
@@ -4016,12 +3902,6 @@
       <c r="F76" t="s">
         <v>59</v>
       </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
       <c r="I76">
         <v>5.5</v>
       </c>
@@ -4472,24 +4352,6 @@
       <c r="F88" t="s">
         <v>109</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88">
-        <v>0</v>
-      </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
-      <c r="M88">
-        <v>0</v>
-      </c>
-      <c r="N88">
-        <v>0</v>
-      </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -4516,17 +4378,11 @@
       <c r="H89">
         <v>6</v>
       </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
       <c r="L89">
         <v>6.5</v>
       </c>
       <c r="M89">
         <v>5.5</v>
-      </c>
-      <c r="N89">
-        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
@@ -4586,12 +4442,6 @@
       <c r="F91" t="s">
         <v>107</v>
       </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
       <c r="I91">
         <v>6.5</v>
       </c>
@@ -5050,9 +4900,6 @@
       <c r="H104">
         <v>6</v>
       </c>
-      <c r="I104">
-        <v>0</v>
-      </c>
       <c r="M104">
         <v>6.5</v>
       </c>
@@ -5117,9 +4964,6 @@
       <c r="G106">
         <v>6.5</v>
       </c>
-      <c r="H106">
-        <v>0</v>
-      </c>
       <c r="I106">
         <v>8</v>
       </c>
@@ -5534,21 +5378,6 @@
       <c r="F118" t="s">
         <v>133</v>
       </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
-      <c r="I118">
-        <v>0</v>
-      </c>
-      <c r="M118">
-        <v>0</v>
-      </c>
-      <c r="N118">
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
@@ -5575,9 +5404,6 @@
       <c r="H119">
         <v>6</v>
       </c>
-      <c r="I119">
-        <v>0</v>
-      </c>
       <c r="M119">
         <v>5.5</v>
       </c>
@@ -5641,9 +5467,6 @@
       </c>
       <c r="G121">
         <v>6.5</v>
-      </c>
-      <c r="H121">
-        <v>0</v>
       </c>
       <c r="I121">
         <v>6</v>
@@ -6557,7 +6380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F58114D-B89F-49BC-8528-AAC9A616442E}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>